<commit_message>
fixed mis-labeled chlorophyll column in fix_sation xls template
</commit_message>
<xml_diff>
--- a/templates/FixStationTemplate.xlsx
+++ b/templates/FixStationTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gov\Projects\djangoProject\dart\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6099738-323C-4D25-976B-AAFB3339978D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAAC0B8-446D-4EDF-8BF5-50E4DBC9E9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{90BC93A9-37F2-43F3-8B40-765139D73F8A}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{90BC93A9-37F2-43F3-8B40-765139D73F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="HL_0" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="14">
   <si>
     <t>Bottle ID</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Int Phytopl.</t>
+  </si>
+  <si>
+    <t>Chlorophyll</t>
   </si>
 </sst>
 </file>
@@ -456,23 +459,23 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -510,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>60</v>
       </c>
@@ -541,7 +544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>10</v>
       </c>
@@ -566,7 +569,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>5</v>
       </c>
@@ -597,7 +600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -636,26 +639,26 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>12</v>
@@ -693,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>140</v>
       </c>
@@ -722,7 +725,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>100</v>
       </c>
@@ -747,7 +750,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>75</v>
       </c>
@@ -768,7 +771,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>50</v>
       </c>
@@ -793,7 +796,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>40</v>
       </c>
@@ -818,7 +821,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>30</v>
       </c>
@@ -839,7 +842,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>20</v>
       </c>
@@ -864,7 +867,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>10</v>
       </c>
@@ -889,7 +892,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>5</v>
       </c>
@@ -914,7 +917,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
@@ -957,23 +960,23 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>90</v>
       </c>
@@ -1034,7 +1037,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>50</v>
       </c>
@@ -1055,7 +1058,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>25</v>
       </c>
@@ -1076,7 +1079,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>10</v>
       </c>
@@ -1099,7 +1102,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1122,7 +1125,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1134,7 +1137,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1146,7 +1149,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1158,7 +1161,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1170,7 +1173,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1195,24 +1198,24 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>80</v>
       </c>
@@ -1278,7 +1281,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>70</v>
       </c>
@@ -1302,7 +1305,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>60</v>
       </c>
@@ -1326,7 +1329,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>50</v>
       </c>
@@ -1354,7 +1357,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>40</v>
       </c>
@@ -1378,7 +1381,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>30</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>20</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>10</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>5</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
     </row>
   </sheetData>

</xml_diff>